<commit_message>
remove CDM and revise CDL/CDH assumptions in Austria residential mapping scheme
</commit_message>
<xml_diff>
--- a/res_mapping_schemes/mapping_Austria_RES.xlsx
+++ b/res_mapping_schemes/mapping_Austria_RES.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10914"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37CA0273-6275-6F4D-B103-02F3941EE824}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9613535-B551-DB4D-823A-F2814E2D61AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4220" yWindow="460" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="108">
   <si>
     <t xml:space="preserve">  Non-insulating constr. (e.g. regular brick)/1991 to 2011</t>
   </si>
@@ -237,11 +237,6 @@
   </si>
   <si>
     <t xml:space="preserve">  Other mixed construction/1981 to 1991</t>
-  </si>
-  <si>
-    <t>42% MIX(MUR+W)/LWAL+CDM/H:1
-44% MIX(MUR+W)/LWAL+CDM/H:2
-14% CR/LFINF+CDM/HBET:3-5</t>
   </si>
   <si>
     <t>42% MIX(MUR+W)/LWAL+CDN/H:1
@@ -249,23 +244,9 @@
 14% CR/LFINF+CDN/HBET:3-5</t>
   </si>
   <si>
-    <t>40% W/LWAL+CDM/H:1
-34% W/LWAL+CDM/H:2
-20% W/LWAL+CDM/HBET:3-5
-6% W/LWAL+CDH/HBET:3-5</t>
-  </si>
-  <si>
     <t>40% W/LWAL+CDN/H:1
 34% W/LWAL+CDN/H:2
 26% W/LWAL+CDN/HBET:3-5</t>
-  </si>
-  <si>
-    <t>5% CR+PC/LWAL+CDM/HBET:3-5
-2% CR+PC/LWAL+CDH/HBET:3-5
-5% CR/LWAL+CDM/HBET:3-5
-2% CR/LWAL+CDH/HBET:3-5
-44% CR/LWAL+CDM/H:2
-42% CR/LWAL+CDM/H:1</t>
   </si>
   <si>
     <t>7% CR+PC/LWAL+CDN/HBET:3-5
@@ -274,22 +255,9 @@
 42% CR/LWAL+CDN/H:1</t>
   </si>
   <si>
-    <t>42% W/LWAL+CDM/H:1
-44% W/LWAL+CDM/H:2
-10% W/LWAL+CDM/HBET:3-5
-4% W/LWAL+CDH/HBET:3-5</t>
-  </si>
-  <si>
     <t>42% W/LWAL+CDN/H:1
 44% W/LWAL+CDN/H:2
 14% W/LWAL+CDN/HBET:3-5</t>
-  </si>
-  <si>
-    <t>30% MIX(MUR+W)/LWAL+CDM/H:1
-24% MIX(MUR+W)/LWAL+CDM/H:2
-30% CR/LFINF+CDM/HBET:3-5
-13% CR/LFINF+CDM/HBET:6-
-3% CR/LFINF+CDH/HBET:6-</t>
   </si>
   <si>
     <t>30% MIX(MUR+W)/LWAL+CDN/H:1
@@ -304,23 +272,6 @@
 22% CR/LFINF+CDN/HBET:6-</t>
   </si>
   <si>
-    <t>28% MIX(MUR+W)/LWAL+CDM/H:1
-20% MIX(MUR+W)/LWAL+CDM/H:2
-30% CR/LFINF+CDM/HBET:3-5
-16% CR/LFINF+CDM/HBET:6-
-6% CR/LFINF+CDH/HBET:6-</t>
-  </si>
-  <si>
-    <t>22% CR+PC/LWAL+CDM/HBET:3-5
-1% CR+PC/LWAL+CDH/HBET:3-5
-37% CR+PC/LWAL+CDM/HBET:6-
-18% CR+PC/LWAL+CDH/HBET:6-
-12% CR/LWAL+CDM/HBET:3-5
-8% CR/LWAL+CDM/HBET:6-
-1% CR/LWAL+CDH/HBET:3-5
-1% CR/LWAL+CDH/HBET:6-</t>
-  </si>
-  <si>
     <t>11% CR+PC/LWAL+CDN/HBET:3-5
 36% CR+PC/LWAL+CDN/HBET:6-
 13% CR/LWAL+CDN/HBET:3-5
@@ -333,34 +284,16 @@
 26% CR/LFINF+CDN/HBET:3-5</t>
   </si>
   <si>
-    <t>5% MUR+CL/LWAL+CDN/H:1
-5% MUR+CL/LWAL+CDN/H:2
-54% CR/LFINF+CDM/HBET:3-5
-23% CR/LFINF+CDM/HBET:6-
-13% CR/LFINF+CDH/HBET:6-</t>
-  </si>
-  <si>
     <t>30% MUR+CL/LWAL+CDN/H:1
 20% MUR+CL/LWAL+CDN/H:2
 29% CR/LFINF+CDN/HBET:3-5
 21% CR/LFINF+CDN/HBET:6-</t>
   </si>
   <si>
-    <t>42% MUR+CL/LWAL+CDN/H:1
-44% MUR+CL/LWAL+CDN/H:2
-14% CR/LFINF+CDM/HBET:3-5</t>
-  </si>
-  <si>
     <t>100% MIX/LH+CDN/H:2</t>
   </si>
   <si>
     <t>100% MUR+CL/LWAL+CDN/H:2</t>
-  </si>
-  <si>
-    <t>100% MIX/LH+CDM/H:2</t>
-  </si>
-  <si>
-    <t>100% CR/LFINF+CDM/HBET:3-5</t>
   </si>
   <si>
     <t>30% MUR+CL/LWAL+CDN/H:1
@@ -402,15 +335,6 @@
   </si>
   <si>
     <t>100% CR/LFINF+CDL/HBET:3-5</t>
-  </si>
-  <si>
-    <t>5% MUR+CL/LWAL+CDN/H:1
-5% CR/LFINF+CDN/H:2
-40% CR/LFINF+CDM/HBET:6-
-50% CR/LFINF+CDM/HBET:3-5</t>
-  </si>
-  <si>
-    <t>100% CR/LFINF+CDM/H:2</t>
   </si>
   <si>
     <t>42% MUR+CL/LWAL+CDN/H:1
@@ -443,14 +367,94 @@
   <si>
     <t>Material and year of construction</t>
   </si>
+  <si>
+    <t>22% CR+PC/LWAL+CDL/HBET:3-5
+1% CR+PC/LWAL+CDH/HBET:3-5
+37% CR+PC/LWAL+CDL/HBET:6-
+18% CR+PC/LWAL+CDH/HBET:6-
+12% CR/LWAL+CDL/HBET:3-5
+8% CR/LWAL+CDL/HBET:6-
+1% CR/LWAL+CDH/HBET:3-5
+1% CR/LWAL+CDH/HBET:6-</t>
+  </si>
+  <si>
+    <t>5% MUR+CL/LWAL+CDN/H:1
+5% CR/LFINF+CDN/H:2
+30% CR/LFINF+CDL/HBET:6-
+35% CR/LFINF+CDL/HBET:3-5
+10% CR/LFINF+CDH/HBET:6-
+15% CR/LFINF+CDH/HBET:3-5</t>
+  </si>
+  <si>
+    <t>30% W/LWAL+CDL/H:1
+10% W/LWAL+CDH/H:1
+24% W/LWAL+CDL/H:2
+10% W/LWAL+CDH/H:2
+20% W/LWAL+CDL/HBET:3-5
+6% W/LWAL+CDH/HBET:3-5</t>
+  </si>
+  <si>
+    <t>75% CR/LFINF+CDL/HBET:3-5
+25% CR/LFINF+CDH/HBET:3-5</t>
+  </si>
+  <si>
+    <t>5% MUR+CL/LWAL+CDN/H:1
+5% MUR+CL/LWAL+CDN/H:2
+54% CR/LFINF+CDL/HBET:3-5
+23% CR/LFINF+CDL/HBET:6-
+13% CR/LFINF+CDH/HBET:6-</t>
+  </si>
+  <si>
+    <t>28% MIX(MUR+W)/LWAL+CDL/H:1
+20% MIX(MUR+W)/LWAL+CDL/H:2
+30% CR/LFINF+CDL/HBET:3-5
+16% CR/LFINF+CDL/HBET:6-
+6% CR/LFINF+CDH/HBET:6-</t>
+  </si>
+  <si>
+    <t>30% MIX(MUR+W)/LWAL+CDL/H:1
+24% MIX(MUR+W)/LWAL+CDL/H:2
+30% CR/LFINF+CDL/HBET:3-5
+13% CR/LFINF+CDL/HBET:6-
+3% CR/LFINF+CDH/HBET:6-</t>
+  </si>
+  <si>
+    <t>42% MUR+CL/LWAL+CDN/H:1
+44% MUR+CL/LWAL+CDN/H:2
+14% CR/LFINF+CDL/HBET:3-5</t>
+  </si>
+  <si>
+    <t>42% W/LWAL+CDL/H:1
+44% W/LWAL+CDL/H:2
+10% W/LWAL+CDL/HBET:3-5
+4% W/LWAL+CDH/HBET:3-5</t>
+  </si>
+  <si>
+    <t>5% CR+PC/LWAL+CDL/HBET:3-5
+2% CR+PC/LWAL+CDH/HBET:3-5
+5% CR/LWAL+CDL/HBET:3-5
+2% CR/LWAL+CDH/HBET:3-5
+44% CR/LWAL+CDL/H:2
+42% CR/LWAL+CDL/H:1</t>
+  </si>
+  <si>
+    <t>100% CR/LFINF+CDL/H:2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -505,17 +509,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -799,7 +806,7 @@
   <dimension ref="A1:BU2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -813,7 +820,7 @@
   <sheetData>
     <row r="1" spans="1:73" s="2" customFormat="1" ht="64.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -1034,221 +1041,221 @@
     </row>
     <row r="2" spans="1:73" s="2" customFormat="1" ht="136" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="I2" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AN2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AO2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AP2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AR2" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AS2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AT2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AU2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AV2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AW2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AX2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AY2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AZ2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="BA2" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="BB2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="BC2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="BD2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="BE2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="BF2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="BG2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="BH2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="BI2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="BJ2" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="BK2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="BL2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="BM2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="BN2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="BO2" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="BP2" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="BQ2" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="BR2" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="BS2" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="P2" s="3" t="s">
+      <c r="BT2" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="Q2" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="AG2" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="AH2" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="AI2" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="AJ2" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="AK2" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="AL2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="AM2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="AN2" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="AO2" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="AP2" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="AQ2" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="AR2" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="AS2" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="AT2" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="AU2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="AV2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="AW2" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="AX2" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="AY2" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="AZ2" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="BA2" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="BB2" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="BC2" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="BD2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="BE2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="BF2" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="BG2" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="BH2" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="BI2" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="BJ2" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="BK2" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="BL2" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="BM2" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="BN2" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="BO2" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="BP2" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="BQ2" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="BR2" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="BS2" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="BT2" s="3" t="s">
-        <v>99</v>
-      </c>
       <c r="BU2" s="3" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1261,7 +1268,7 @@
   <dimension ref="A1:BU2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1272,7 +1279,7 @@
   <sheetData>
     <row r="1" spans="1:73" s="2" customFormat="1" ht="64.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -1493,221 +1500,221 @@
     </row>
     <row r="2" spans="1:73" s="2" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="K2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AP2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AR2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AS2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AT2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AU2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AX2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AY2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AZ2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="BA2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="BB2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="BC2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="BD2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="BE2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="BG2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="BH2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="BI2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="BJ2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="BK2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="BL2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="BM2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="BN2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="BO2" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="BP2" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="BQ2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="BR2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="BS2" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="BT2" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="BU2" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="AG2" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="AH2" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="AI2" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="AJ2" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="AK2" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="AL2" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="AM2" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="AN2" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="AO2" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="AP2" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="AQ2" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="AR2" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="AS2" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="AT2" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="AU2" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="AV2" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="AW2" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="AX2" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="AY2" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="AZ2" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="BA2" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="BB2" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="BC2" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="BD2" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="BE2" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="BF2" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="BG2" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="BH2" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="BI2" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="BJ2" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="BK2" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="BL2" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="BM2" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="BN2" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="BO2" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="BP2" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="BQ2" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="BR2" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="BS2" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="BT2" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="BU2" s="3" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>